<commit_message>
Updated FI MC and Neon scripts
</commit_message>
<xml_diff>
--- a/docs/Examples/Fluid_Inclusions/Fluid_Inclusion_Data.xlsx
+++ b/docs/Examples/Fluid_Inclusions/Fluid_Inclusion_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Fluid_Inclusions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AB8C69-D2D4-4807-B2F7-3AF02F290035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B9CBDB-937D-4AAF-96CF-D2AC888B842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{2E7CFF85-7259-4F73-94DE-91E9C7FABD09}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sample</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Density_g_cm3</t>
+  </si>
+  <si>
+    <t>Corrected_Splitting</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48BFBA5-F5FB-4629-A716-7FB1DCE197C5}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,7 +458,7 @@
     <col min="3" max="3" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +468,11 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -476,8 +482,11 @@
       <c r="C2">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -487,8 +496,11 @@
       <c r="C3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,8 +510,11 @@
       <c r="C4">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>103.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -509,8 +524,11 @@
       <c r="C5">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -520,8 +538,11 @@
       <c r="C6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -531,8 +552,11 @@
       <c r="C7">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>104.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -542,8 +566,11 @@
       <c r="C8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>105.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -553,8 +580,11 @@
       <c r="C9">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -564,8 +594,11 @@
       <c r="C10">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -575,8 +608,11 @@
       <c r="C11">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>103.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -585,6 +621,9 @@
       </c>
       <c r="C12">
         <v>0.33</v>
+      </c>
+      <c r="D12">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>